<commit_message>
Updated data and README.
</commit_message>
<xml_diff>
--- a/Data/NF_Model Parameters.xlsx
+++ b/Data/NF_Model Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom Kelly\Dropbox\Documents\BTE\Yingling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DFBF7D-4AC2-47E1-A77B-7AFD04863EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79C08E3-96F4-40FC-BC0B-7BC824267BE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A04AC130-C96E-402F-9A4C-72420F5646D0}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="23040" windowHeight="12372" xr2:uid="{A04AC130-C96E-402F-9A4C-72420F5646D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
   <si>
     <t>Param</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>E_OTHER</t>
+  </si>
+  <si>
+    <t>log</t>
   </si>
 </sst>
 </file>
@@ -745,23 +748,23 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="19"/>
+    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="23" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -787,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -808,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -834,7 +837,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -860,7 +863,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -886,7 +889,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -910,7 +913,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -936,9 +939,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="C8" s="23">
         <f>LOG(0.0885)</f>
@@ -959,7 +965,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -979,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>54</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>55</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>56</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>57</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>58</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>59</v>
       </c>
@@ -1301,7 +1307,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
@@ -1321,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>22</v>
       </c>
@@ -1347,7 +1353,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>23</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>24</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>25</v>
       </c>
@@ -1423,7 +1429,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>26</v>
       </c>
@@ -1449,7 +1455,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>27</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>28</v>
       </c>
@@ -1492,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>30</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>31</v>
       </c>
@@ -1570,7 +1576,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>32</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>33</v>
       </c>
@@ -1620,7 +1626,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>34</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="15" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>35</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
         <v>36</v>
       </c>
@@ -1689,7 +1695,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>38</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
         <v>39</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>40</v>
       </c>
@@ -1791,7 +1797,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>41</v>
       </c>
@@ -1814,7 +1820,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="16" t="s">
         <v>42</v>
       </c>

</xml_diff>